<commit_message>
updated burndown, backlog, and post production docs
</commit_message>
<xml_diff>
--- a/Docs/Burndown Charts.xlsx
+++ b/Docs/Burndown Charts.xlsx
@@ -5,11 +5,11 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\315\p2\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\315\project2\CSCE315-Project2\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
   <si>
     <t>Task</t>
   </si>
@@ -188,7 +188,64 @@
     <t>0-5 days</t>
   </si>
   <si>
-    <t>kjfa;jslkjfd</t>
+    <t>Update Board-Game Layout</t>
+  </si>
+  <si>
+    <t>GUI Client: Connecting to server</t>
+  </si>
+  <si>
+    <t>GUI Client: Sending move to server</t>
+  </si>
+  <si>
+    <t>GUI Client: Interpret server responses</t>
+  </si>
+  <si>
+    <t>GUI Client: Display board</t>
+  </si>
+  <si>
+    <t>GUI Client: Testing user access</t>
+  </si>
+  <si>
+    <t>GUI Client: Added images</t>
+  </si>
+  <si>
+    <t>GUI Client: Added buttons</t>
+  </si>
+  <si>
+    <t>GUI Client: Update Color Scheme</t>
+  </si>
+  <si>
+    <t>GUI Client: Improve efficiency</t>
+  </si>
+  <si>
+    <t>GUI Client: Added functionality to buttons</t>
+  </si>
+  <si>
+    <t>GUI Client: Updated connection issues</t>
+  </si>
+  <si>
+    <t>GUI Client: Password screen</t>
+  </si>
+  <si>
+    <t>GUI Client: Centering client</t>
+  </si>
+  <si>
+    <t>GUI Client: Connection functionality</t>
+  </si>
+  <si>
+    <t>GUI Client: Allow insensitive password</t>
+  </si>
+  <si>
+    <t>Perfect Command Transcribing</t>
+  </si>
+  <si>
+    <t>Creation of GUI Class</t>
+  </si>
+  <si>
+    <t>GUI Client: Fix functionality of buttons</t>
+  </si>
+  <si>
+    <t>GUI Client: Fixed row and columns</t>
   </si>
 </sst>
 </file>
@@ -238,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -418,13 +475,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -485,7 +551,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -568,13 +637,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF3F3F3F"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FFA5A5A5"/>
         </left>
@@ -598,6 +660,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -773,13 +842,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FF8F8F8F"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF8F8F8F"/>
@@ -802,6 +864,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF8F8F8F"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1727,6 +1796,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1994,11 +2064,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="192345328"/>
-        <c:axId val="192345888"/>
+        <c:axId val="179950400"/>
+        <c:axId val="179950960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="192345328"/>
+        <c:axId val="179950400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2088,7 +2158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192345888"/>
+        <c:crossAx val="179950960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2096,7 +2166,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="192345888"/>
+        <c:axId val="179950960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2161,7 +2231,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192345328"/>
+        <c:crossAx val="179950400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -2177,6 +2247,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2595,11 +2666,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="192341408"/>
-        <c:axId val="191660048"/>
+        <c:axId val="177992976"/>
+        <c:axId val="177993536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="192341408"/>
+        <c:axId val="177992976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2689,7 +2760,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="191660048"/>
+        <c:crossAx val="177993536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2697,7 +2768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191660048"/>
+        <c:axId val="177993536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2762,7 +2833,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="192341408"/>
+        <c:crossAx val="177992976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -2887,7 +2958,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 2</a:t>
+              <a:t> 3</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2962,10 +3033,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sprint3!$C$28:$C$40</c:f>
+              <c:f>Sprint3!$C$28:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2983,42 +3054,33 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint3!$D$28:$D$40</c:f>
+              <c:f>Sprint3!$D$28:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3059,10 +3121,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sprint3!$C$28:$C$40</c:f>
+              <c:f>Sprint3!$C$28:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3080,75 +3142,33 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint3!$E$28:$E$40</c:f>
+              <c:f>Sprint3!$E$28:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3164,11 +3184,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="356970784"/>
-        <c:axId val="356971344"/>
+        <c:axId val="181188208"/>
+        <c:axId val="181188768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="356970784"/>
+        <c:axId val="181188208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3258,7 +3278,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="356971344"/>
+        <c:crossAx val="181188768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3266,7 +3286,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="356971344"/>
+        <c:axId val="181188768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3331,7 +3351,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="356970784"/>
+        <c:crossAx val="181188208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2"/>
@@ -3410,7 +3430,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter>
-      <c:oddHeader>&amp;CSprint 1</c:oddHeader>
+      <c:oddHeader>&amp;C&amp;26Sprint 3</c:oddHeader>
     </c:headerFooter>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup orientation="landscape"/>
@@ -5347,8 +5367,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table146" displayName="Table146" ref="C27:E40" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
-  <autoFilter ref="C27:E40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table146" displayName="Table146" ref="C27:E33" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="C27:E33"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Time Spent" dataDxfId="8"/>
     <tableColumn id="2" name="Ideal Backlog" dataDxfId="7">
@@ -5363,8 +5383,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table257" displayName="Table257" ref="A1:B3" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3">
-  <autoFilter ref="A1:B3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table257" displayName="Table257" ref="A1:B21" totalsRowShown="0" headerRowDxfId="5" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2">
+  <autoFilter ref="A1:B21"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Task" dataDxfId="1"/>
     <tableColumn id="2" name="Time Finished" dataDxfId="0"/>
@@ -6482,7 +6502,7 @@
   </sheetPr>
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A2" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -6867,7 +6887,7 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -7298,8 +7318,8 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7321,93 +7341,167 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B2" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="10"/>
+        <v>71</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
+      <c r="A10" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="19"/>
+      <c r="A18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
+      <c r="A19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
+      <c r="A20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
@@ -7445,11 +7539,10 @@
       </c>
       <c r="D28" s="15">
         <f>COUNT(Table257[Time Finished])</f>
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E28" s="16">
-        <f>25-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -7458,12 +7551,10 @@
         <v>1</v>
       </c>
       <c r="D29" s="15">
-        <f>ROUNDUP(25-(25/12*C29),0)</f>
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E29" s="16">
-        <f>E28-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -7471,10 +7562,11 @@
         <f t="shared" ref="C30:C37" si="0">C29+1</f>
         <v>2</v>
       </c>
-      <c r="D30" s="15"/>
+      <c r="D30" s="15">
+        <v>12</v>
+      </c>
       <c r="E30" s="16">
-        <f>E29-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -7482,10 +7574,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D31" s="15"/>
+      <c r="D31" s="15">
+        <v>8</v>
+      </c>
       <c r="E31" s="16">
-        <f>E30-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -7493,10 +7586,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D32" s="15"/>
+      <c r="D32" s="15">
+        <v>4</v>
+      </c>
       <c r="E32" s="16">
-        <f>E31-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.2">
@@ -7504,10 +7598,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D33" s="15"/>
+      <c r="D33" s="15">
+        <v>0</v>
+      </c>
       <c r="E33" s="16">
-        <f>E32-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.2">
@@ -7518,7 +7613,7 @@
       <c r="D34" s="15"/>
       <c r="E34" s="16">
         <f>E33-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.2">
@@ -7529,7 +7624,7 @@
       <c r="D35" s="15"/>
       <c r="E35" s="16">
         <f>E34-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.2">
@@ -7540,7 +7635,7 @@
       <c r="D36" s="15"/>
       <c r="E36" s="16">
         <f>E35-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.2">
@@ -7551,7 +7646,7 @@
       <c r="D37" s="15"/>
       <c r="E37" s="16">
         <f>E36-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.2">
@@ -7561,7 +7656,7 @@
       <c r="D38" s="15"/>
       <c r="E38" s="16">
         <f>E37-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.2">
@@ -7571,7 +7666,7 @@
       <c r="D39" s="15"/>
       <c r="E39" s="16">
         <f>E38-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.2">
@@ -7581,14 +7676,14 @@
       <c r="D40" s="15"/>
       <c r="E40" s="16">
         <f>E39-COUNTIF(Table257[Time Finished],Table146[[#This Row],[Time Spent]])</f>
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;26Sprint 2</oddHeader>
+    <oddHeader>&amp;C&amp;26Sprint 3</oddHeader>
   </headerFooter>
   <drawing r:id="rId2"/>
   <tableParts count="2">

</xml_diff>